<commit_message>
add tests for property buildings and some methods for testAutoKufar
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -10,13 +10,14 @@
     <sheet name="citySelection" sheetId="3" r:id="rId6"/>
     <sheet name="Calculator" sheetId="4" r:id="rId7"/>
     <sheet name="listItemsForSearch" sheetId="5" r:id="rId8"/>
-    <sheet name="Data" sheetId="6" r:id="rId9"/>
+    <sheet name="listBuildings" sheetId="6" r:id="rId9"/>
+    <sheet name="Data" sheetId="7" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="194">
   <si>
     <t>Документ был экспортирован из Numbers. Каждая таблица была конвертирована в рабочий лист Excel. Все другие объекты на листах Numbers были помещены на отдельные рабочие листы. Имейте в виду, что расчеты формул могут отличаться от расчетов в Excel.</t>
   </si>
@@ -495,6 +496,54 @@
   </si>
   <si>
     <t>Смеситель</t>
+  </si>
+  <si>
+    <t>listBuildings</t>
+  </si>
+  <si>
+    <t>propertyType</t>
+  </si>
+  <si>
+    <t>PT001</t>
+  </si>
+  <si>
+    <t>Новостройки</t>
+  </si>
+  <si>
+    <t>PT002</t>
+  </si>
+  <si>
+    <t>Квартиры</t>
+  </si>
+  <si>
+    <t>PT003</t>
+  </si>
+  <si>
+    <t>Комнаты</t>
+  </si>
+  <si>
+    <t>PT004</t>
+  </si>
+  <si>
+    <t>Дома, коттеджи</t>
+  </si>
+  <si>
+    <t>PT005</t>
+  </si>
+  <si>
+    <t>Гаражи и стоянки</t>
+  </si>
+  <si>
+    <t>PT006</t>
+  </si>
+  <si>
+    <t>Участки</t>
+  </si>
+  <si>
+    <t>PT007</t>
+  </si>
+  <si>
+    <t>Коммерческая</t>
   </si>
   <si>
     <t>TestTitle</t>
@@ -635,7 +684,7 @@
       <name val="Menlo Regular"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +742,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="24"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="25"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1101,7 +1156,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1282,16 +1337,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="9" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1340,6 +1404,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa2bd90"/>
       <rgbColor rgb="ff99cc00"/>
     </indexedColors>
@@ -2618,7 +2683,7 @@
     </row>
     <row r="19">
       <c r="B19" t="s" s="3">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2629,6 +2694,22 @@
         <v>5</v>
       </c>
       <c r="D20" t="s" s="5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="4"/>
+      <c r="C22" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s" s="5">
         <v>12</v>
       </c>
     </row>
@@ -2648,7 +2729,8 @@
     <hyperlink ref="D14" location="'citySelection'!R1C1" tooltip="" display="citySelection"/>
     <hyperlink ref="D16" location="'Calculator'!R1C1" tooltip="" display="Calculator"/>
     <hyperlink ref="D18" location="'listItemsForSearch'!R1C1" tooltip="" display="listItemsForSearch"/>
-    <hyperlink ref="D20" location="'Data'!R1C1" tooltip="" display="Data"/>
+    <hyperlink ref="D20" location="'listBuildings'!R1C1" tooltip="" display="listBuildings"/>
+    <hyperlink ref="D22" location="'Data'!R1C1" tooltip="" display="Data"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3712,266 +3794,380 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="3" width="16.3516" style="59" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="32">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s" s="33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" customHeight="1">
+      <c r="A2" t="s" s="60">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s" s="54">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s" s="55">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" ht="12.9" customHeight="1">
+      <c r="A3" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s" s="57">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s" s="58">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" ht="12.9" customHeight="1">
+      <c r="A4" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s" s="57">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s" s="58">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" ht="12.9" customHeight="1">
+      <c r="A5" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="57">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s" s="58">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" ht="12.9" customHeight="1">
+      <c r="A6" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="57">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s" s="58">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" ht="12.9" customHeight="1">
+      <c r="A7" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="57">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s" s="58">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" ht="12.9" customHeight="1">
+      <c r="A8" t="s" s="61">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="57">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s" s="58">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.17188" style="59" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="59" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="59" customWidth="1"/>
-    <col min="4" max="4" width="20.3516" style="59" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="59" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="59" customWidth="1"/>
+    <col min="1" max="1" width="7.17188" style="62" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="62" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="62" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="62" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="60">
+      <c r="A1" t="s" s="63">
         <v>14</v>
       </c>
-      <c r="B1" t="s" s="61">
+      <c r="B1" t="s" s="64">
         <v>15</v>
       </c>
-      <c r="C1" t="s" s="61">
-        <v>149</v>
-      </c>
-      <c r="D1" t="s" s="61">
-        <v>150</v>
-      </c>
-      <c r="E1" s="62"/>
+      <c r="C1" t="s" s="64">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s" s="64">
+        <v>166</v>
+      </c>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s" s="64">
-        <v>151</v>
-      </c>
-      <c r="C2" t="s" s="65">
-        <v>152</v>
-      </c>
-      <c r="D2" t="s" s="65">
-        <v>153</v>
+      <c r="A2" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s" s="67">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s" s="68">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s" s="68">
+        <v>169</v>
       </c>
       <c r="E2" s="27"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s" s="66">
-        <v>154</v>
-      </c>
-      <c r="C3" t="s" s="67">
-        <v>155</v>
-      </c>
-      <c r="D3" t="s" s="67">
-        <v>156</v>
+      <c r="A3" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s" s="69">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s" s="70">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s" s="70">
+        <v>172</v>
       </c>
       <c r="E3" s="27"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s" s="66">
-        <v>157</v>
-      </c>
-      <c r="C4" t="s" s="67">
-        <v>158</v>
-      </c>
-      <c r="D4" t="s" s="67">
-        <v>159</v>
+      <c r="A4" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s" s="69">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s" s="70">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s" s="70">
+        <v>175</v>
       </c>
       <c r="E4" s="27"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="66">
-        <v>160</v>
-      </c>
-      <c r="C5" t="s" s="67">
-        <v>161</v>
-      </c>
-      <c r="D5" t="s" s="67">
-        <v>162</v>
+      <c r="A5" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="69">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s" s="70">
+        <v>177</v>
+      </c>
+      <c r="D5" t="s" s="70">
+        <v>178</v>
       </c>
       <c r="E5" s="27"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s" s="66">
-        <v>163</v>
-      </c>
-      <c r="C6" t="s" s="67">
-        <v>164</v>
-      </c>
-      <c r="D6" t="s" s="67">
-        <v>165</v>
+      <c r="A6" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="69">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s" s="70">
+        <v>180</v>
+      </c>
+      <c r="D6" t="s" s="70">
+        <v>181</v>
       </c>
       <c r="E6" s="27"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s" s="66">
-        <v>166</v>
-      </c>
-      <c r="C7" t="s" s="67">
-        <v>167</v>
-      </c>
-      <c r="D7" t="s" s="67">
-        <v>168</v>
+      <c r="A7" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="69">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s" s="70">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s" s="70">
+        <v>184</v>
       </c>
       <c r="E7" s="27"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s" s="66">
-        <v>169</v>
-      </c>
-      <c r="C8" t="s" s="67">
-        <v>170</v>
-      </c>
-      <c r="D8" t="s" s="67">
-        <v>171</v>
+      <c r="A8" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="69">
+        <v>185</v>
+      </c>
+      <c r="C8" t="s" s="70">
+        <v>186</v>
+      </c>
+      <c r="D8" t="s" s="70">
+        <v>187</v>
       </c>
       <c r="E8" s="27"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s" s="66">
-        <v>172</v>
-      </c>
-      <c r="C9" t="s" s="67">
-        <v>173</v>
-      </c>
-      <c r="D9" t="s" s="67">
-        <v>174</v>
+      <c r="A9" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s" s="69">
+        <v>188</v>
+      </c>
+      <c r="C9" t="s" s="70">
+        <v>189</v>
+      </c>
+      <c r="D9" t="s" s="70">
+        <v>190</v>
       </c>
       <c r="E9" s="27"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="63">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s" s="66">
-        <v>175</v>
-      </c>
-      <c r="C10" t="s" s="67">
-        <v>176</v>
-      </c>
-      <c r="D10" t="s" s="67">
-        <v>177</v>
+      <c r="A10" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s" s="69">
+        <v>191</v>
+      </c>
+      <c r="C10" t="s" s="70">
+        <v>192</v>
+      </c>
+      <c r="D10" t="s" s="70">
+        <v>193</v>
       </c>
       <c r="E10" s="27"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" s="47"/>
       <c r="B11" s="27"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="27"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" s="27"/>
       <c r="B12" s="27"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="27"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" s="27"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="27"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" s="27"/>
       <c r="B14" s="27"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="27"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" s="27"/>
       <c r="B15" s="27"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="27"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" s="27"/>
       <c r="B16" s="27"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="27"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" s="27"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="27"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" s="27"/>
       <c r="B18" s="27"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="27"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="27"/>
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="27"/>
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="27"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="27"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
       <c r="E23" s="27"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="27"/>
     </row>
   </sheetData>

</xml_diff>